<commit_message>
legal terms and others
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,40 +4,29 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Students app" sheetId="1" r:id="rId1"/>
-    <sheet name="Admin tool" sheetId="2" r:id="rId2"/>
+    <sheet name="Teacher app" sheetId="2" r:id="rId2"/>
+    <sheet name="Others" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>joining class with Barcode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>change UI skin/theme</t>
   </si>
   <si>
-    <t>student request to join a class</t>
-  </si>
-  <si>
     <t>auto-approve and manual approve setting</t>
   </si>
   <si>
-    <t>reply back private message</t>
-  </si>
-  <si>
     <t>randomly generate pseudo exams</t>
   </si>
   <si>
-    <t>support written exercises</t>
-  </si>
-  <si>
     <t>save a message in Inbox</t>
   </si>
   <si>
@@ -48,14 +37,133 @@
   </si>
   <si>
     <t xml:space="preserve">share notification or private messages to others thru 3rd party SNS/Email, etc. </t>
+  </si>
+  <si>
+    <t>upload course video</t>
+  </si>
+  <si>
+    <t>access to course video</t>
+  </si>
+  <si>
+    <t>joining class with QR code</t>
+  </si>
+  <si>
+    <t>smart exercises (scanned to pdf) imported thru modular scan</t>
+  </si>
+  <si>
+    <t>several teachers can contribute to exercises of a course (e.g. A 1.1) together</t>
+  </si>
+  <si>
+    <t>registrated students can access to legacy problem sets</t>
+  </si>
+  <si>
+    <t>when a student enrolls to another course, he can still access to the exercises he has done before</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>sign in with 3rd party account (e.g. wechat, sina, qq)</t>
+  </si>
+  <si>
+    <t>answer questions from students to a specific question</t>
+  </si>
+  <si>
+    <t>useful for students who do not adopt the app. A way to promote the app between students</t>
+  </si>
+  <si>
+    <t>student not enrolled the class can request to join it</t>
+  </si>
+  <si>
+    <t>reply back private message sent from teacher</t>
+  </si>
+  <si>
+    <t>support written exercises 写作题</t>
+  </si>
+  <si>
+    <t>provide course material or summary</t>
+  </si>
+  <si>
+    <t>to provide more detailed explanation. For Q &amp; A students can ask general questions</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>allow student to ask question to teacher for a specific problem (e.g. discussion thread)</t>
+  </si>
+  <si>
+    <t>rich version with full features</t>
+  </si>
+  <si>
+    <t>expand to other languages</t>
+  </si>
+  <si>
+    <t>paid version and target large teacher/students ratio (e.g. institute)</t>
+  </si>
+  <si>
+    <t>provide description for course sequence content</t>
+  </si>
+  <si>
+    <t>allow students to have a summary for what a sequence teachs. 每节课的教育重点</t>
+  </si>
+  <si>
+    <t>oral exercises with student 1:1 thru audio</t>
+  </si>
+  <si>
+    <t>oral exercises with student 1:n thru audio</t>
+  </si>
+  <si>
+    <t>oral exercises with student 1:1 thru video</t>
+  </si>
+  <si>
+    <t>oral exercises with student 1:n thru video</t>
+  </si>
+  <si>
+    <t>oral exercises 口试 1: n thru audio</t>
+  </si>
+  <si>
+    <t>oral exercises 口试 1:1 thru audio</t>
+  </si>
+  <si>
+    <t>oral exercises 口试 1: n thru video</t>
+  </si>
+  <si>
+    <t>oral exercises 口试 1: 1 thru video</t>
+  </si>
+  <si>
+    <t>useful to correct 发音的口型</t>
+  </si>
+  <si>
+    <t>Could be free to download (e.g. independent teachers)</t>
+  </si>
+  <si>
+    <t>public  version with limited features</t>
+  </si>
+  <si>
+    <t>data analysis modula</t>
+  </si>
+  <si>
+    <t>compare exercises results with differet classes</t>
+  </si>
+  <si>
+    <t>sceario like a/b testing to verify 教改</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,8 +191,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,60 +503,221 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -450,27 +725,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first level UI options
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>change UI skin/theme</t>
   </si>
@@ -157,6 +157,51 @@
   </si>
   <si>
     <t>bad UX for big table format on small form factor phones need to separate to several small tables instead?</t>
+  </si>
+  <si>
+    <t>edit QA</t>
+  </si>
+  <si>
+    <t>delete QA</t>
+  </si>
+  <si>
+    <t>create class</t>
+  </si>
+  <si>
+    <t>save messsange and sent later</t>
+  </si>
+  <si>
+    <t>publish message directly</t>
+  </si>
+  <si>
+    <t>for this version, admin needs to click "Save" then the button "publish" will display</t>
+  </si>
+  <si>
+    <t>show ranking against other students in the same class based on the score</t>
+  </si>
+  <si>
+    <t>encourage students to redo quizs if score is low</t>
+  </si>
+  <si>
+    <t>show answers to quiz after certain periods</t>
+  </si>
+  <si>
+    <t>schedule when to post answers to students</t>
+  </si>
+  <si>
+    <t>teach could auto-schedule to post answers to a test at a certain time</t>
+  </si>
+  <si>
+    <t>add sample answer to a problem</t>
+  </si>
+  <si>
+    <t>this is to help students how to answer a quiz</t>
+  </si>
+  <si>
+    <t>add answers to a quiz</t>
+  </si>
+  <si>
+    <t>get credits when playing exercises</t>
   </si>
 </sst>
 </file>
@@ -512,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,6 +695,24 @@
         <v>46</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -658,16 +721,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -708,7 +771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -740,6 +803,55 @@
       </c>
       <c r="B12" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>